<commit_message>
infinite scroll, database search bug fixed
</commit_message>
<xml_diff>
--- a/database/power-cur.xlsx
+++ b/database/power-cur.xlsx
@@ -14,204 +14,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>시간</t>
   </si>
   <si>
-    <t>순시전력량(kW)</t>
-  </si>
-  <si>
-    <t>2015-09-09 11:10</t>
-  </si>
-  <si>
-    <t>2015-09-09 11:00</t>
-  </si>
-  <si>
-    <t>2015-09-09 10:50</t>
-  </si>
-  <si>
-    <t>2015-09-09 10:40</t>
-  </si>
-  <si>
-    <t>2015-09-09 10:20</t>
-  </si>
-  <si>
-    <t>2015-09-08 12:50</t>
-  </si>
-  <si>
-    <t>2015-09-08 12:40</t>
-  </si>
-  <si>
-    <t>2015-09-08 12:30</t>
-  </si>
-  <si>
-    <t>2015-09-08 12:20</t>
-  </si>
-  <si>
-    <t>2015-09-08 12:10</t>
-  </si>
-  <si>
-    <t>2015-09-08 12:00</t>
-  </si>
-  <si>
-    <t>2015-09-08 11:50</t>
-  </si>
-  <si>
-    <t>2015-09-08 11:40</t>
-  </si>
-  <si>
-    <t>2015-09-08 11:30</t>
-  </si>
-  <si>
-    <t>2015-09-08 11:20</t>
-  </si>
-  <si>
-    <t>2015-09-08 11:10</t>
-  </si>
-  <si>
-    <t>2015-09-08 11:00</t>
-  </si>
-  <si>
-    <t>2015-09-08 10:50</t>
-  </si>
-  <si>
-    <t>2015-09-08 10:40</t>
-  </si>
-  <si>
-    <t>2015-09-08 10:30</t>
-  </si>
-  <si>
-    <t>2015-09-08 10:20</t>
-  </si>
-  <si>
-    <t>2015-09-08 10:10</t>
-  </si>
-  <si>
-    <t>2015-09-08 10:00</t>
-  </si>
-  <si>
-    <t>2015-09-08 09:50</t>
-  </si>
-  <si>
-    <t>2015-09-08 09:40</t>
-  </si>
-  <si>
-    <t>2015-09-08 09:30</t>
-  </si>
-  <si>
-    <t>2015-09-07 10:20</t>
-  </si>
-  <si>
-    <t>2015-09-07 10:10</t>
-  </si>
-  <si>
-    <t>2015-09-07 10:00</t>
-  </si>
-  <si>
-    <t>2015-09-07 09:50</t>
-  </si>
-  <si>
-    <t>2015-09-07 09:40</t>
-  </si>
-  <si>
-    <t>2015-09-07 09:30</t>
-  </si>
-  <si>
-    <t>2015-09-07 09:20</t>
-  </si>
-  <si>
-    <t>2015-09-07 09:10</t>
-  </si>
-  <si>
-    <t>2015-09-07 09:00</t>
-  </si>
-  <si>
-    <t>2015-09-04 13:30</t>
-  </si>
-  <si>
-    <t>2015-09-04 13:20</t>
-  </si>
-  <si>
-    <t>2015-09-04 13:10</t>
-  </si>
-  <si>
-    <t>2015-09-04 13:00</t>
-  </si>
-  <si>
-    <t>2015-09-04 12:50</t>
-  </si>
-  <si>
-    <t>2015-09-04 12:40</t>
-  </si>
-  <si>
-    <t>2015-09-04 12:30</t>
-  </si>
-  <si>
-    <t>2015-09-04 12:20</t>
-  </si>
-  <si>
-    <t>2015-09-04 12:10</t>
-  </si>
-  <si>
-    <t>2015-09-04 12:00</t>
-  </si>
-  <si>
-    <t>2015-09-04 11:50</t>
-  </si>
-  <si>
-    <t>2015-09-04 11:40</t>
-  </si>
-  <si>
-    <t>2015-09-04 11:30</t>
-  </si>
-  <si>
-    <t>2015-09-03 15:50</t>
-  </si>
-  <si>
-    <t>2015-09-03 15:40</t>
-  </si>
-  <si>
-    <t>2015-09-03 15:30</t>
-  </si>
-  <si>
-    <t>2015-09-03 15:20</t>
-  </si>
-  <si>
-    <t>2015-09-03 15:10</t>
-  </si>
-  <si>
-    <t>2015-09-03 15:00</t>
-  </si>
-  <si>
-    <t>2015-09-03 14:50</t>
-  </si>
-  <si>
-    <t>2015-09-03 14:40</t>
-  </si>
-  <si>
-    <t>2015-09-03 14:30</t>
-  </si>
-  <si>
-    <t>2015-09-03 14:20</t>
-  </si>
-  <si>
-    <t>2015-09-03 14:10</t>
-  </si>
-  <si>
-    <t>2015-09-03 10:50</t>
-  </si>
-  <si>
-    <t>2015-09-03 10:40</t>
-  </si>
-  <si>
-    <t>2015-09-03 10:30</t>
-  </si>
-  <si>
-    <t>2015-09-03 10:20</t>
-  </si>
-  <si>
-    <t>2015-09-03 10:10</t>
+    <t>순시전력(kW)</t>
+  </si>
+  <si>
+    <t>2015-11-18 18:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 18:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 17:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 16:20</t>
+  </si>
+  <si>
+    <t>2015-11-18 16:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 16:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 15:50</t>
+  </si>
+  <si>
+    <t>2015-11-18 15:40</t>
+  </si>
+  <si>
+    <t>2015-11-18 15:30</t>
+  </si>
+  <si>
+    <t>2015-11-18 14:50</t>
+  </si>
+  <si>
+    <t>2015-11-18 14:40</t>
+  </si>
+  <si>
+    <t>2015-11-18 14:30</t>
+  </si>
+  <si>
+    <t>2015-11-18 14:20</t>
+  </si>
+  <si>
+    <t>2015-11-18 14:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 14:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 13:50</t>
+  </si>
+  <si>
+    <t>2015-11-18 13:40</t>
+  </si>
+  <si>
+    <t>2015-11-18 13:30</t>
+  </si>
+  <si>
+    <t>2015-11-18 13:20</t>
+  </si>
+  <si>
+    <t>2015-11-18 13:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 13:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 12:50</t>
+  </si>
+  <si>
+    <t>2015-11-18 12:40</t>
+  </si>
+  <si>
+    <t>2015-11-18 12:30</t>
+  </si>
+  <si>
+    <t>2015-11-18 12:20</t>
+  </si>
+  <si>
+    <t>2015-11-18 12:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 12:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:50</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:40</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:30</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:20</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 11:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:50</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:40</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:30</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:20</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:10</t>
+  </si>
+  <si>
+    <t>2015-11-18 10:00</t>
+  </si>
+  <si>
+    <t>2015-11-18 09:40</t>
   </si>
 </sst>
 </file>
@@ -557,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,7 +508,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -588,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -596,7 +524,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -604,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -612,7 +540,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -620,7 +548,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -628,7 +556,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -636,7 +564,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -644,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -652,7 +580,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -660,7 +588,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -668,7 +596,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -676,7 +604,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -684,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -692,7 +620,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -700,7 +628,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -708,7 +636,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -716,7 +644,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -724,7 +652,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -732,7 +660,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -740,7 +668,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -748,7 +676,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -756,7 +684,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -764,7 +692,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -772,7 +700,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -780,7 +708,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -788,7 +716,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -796,7 +724,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -804,7 +732,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -812,7 +740,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -820,7 +748,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -828,7 +756,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -836,7 +764,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -844,7 +772,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -852,7 +780,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -860,7 +788,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -868,7 +796,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -876,7 +804,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -884,7 +812,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -892,199 +820,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" s="2">
-        <v>0</v>
+        <v>0.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>